<commit_message>
File-Upload y otras cosillas
</commit_message>
<xml_diff>
--- a/node-central/equipos.xlsx
+++ b/node-central/equipos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omega\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7553796-A4E9-43DD-88BF-4196FF2ED8E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27541AB3-6AAC-46DC-B9BF-D57A2565B30F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1126,7 +1126,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P298"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A292" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B138" sqref="B138"/>
     </sheetView>
   </sheetViews>
@@ -16048,6 +16048,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E749FFFE0989D649B56E82565BC24D6D" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1941bbcce4e679288056da6a6786e297">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5c753c04-4c07-4dfb-b25e-c56059ca961d" xmlns:ns3="af8514bc-be7a-429c-a492-f298258d52a7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="17841404dd05f148ab640c9eb1a4253a" ns2:_="" ns3:_="">
     <xsd:import namespace="5c753c04-4c07-4dfb-b25e-c56059ca961d"/>
@@ -16212,36 +16227,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41708F13-A982-4911-B4E6-AD7676D3659D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2274D87C-672A-4E8A-B957-39CF092F5081}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="5c753c04-4c07-4dfb-b25e-c56059ca961d"/>
-    <ds:schemaRef ds:uri="af8514bc-be7a-429c-a492-f298258d52a7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -16264,9 +16253,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2274D87C-672A-4E8A-B957-39CF092F5081}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41708F13-A982-4911-B4E6-AD7676D3659D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="5c753c04-4c07-4dfb-b25e-c56059ca961d"/>
+    <ds:schemaRef ds:uri="af8514bc-be7a-429c-a492-f298258d52a7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>